<commit_message>
cleared data in excel workbook
</commit_message>
<xml_diff>
--- a/ice.xlsx
+++ b/ice.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klarrieu\Desktop\Seb_Class\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8175" windowWidth="11880" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11880" windowHeight="8175"/>
   </bookViews>
   <sheets>
-    <sheet name="menu" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="menu" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Flavors</t>
   </si>
@@ -34,105 +39,56 @@
     <t>vanilla</t>
   </si>
   <si>
-    <t>Barry</t>
-  </si>
-  <si>
-    <t>small</t>
-  </si>
-  <si>
-    <t>1.50</t>
-  </si>
-  <si>
     <t>chocolate</t>
   </si>
   <si>
-    <t>Larry</t>
-  </si>
-  <si>
-    <t>family size</t>
-  </si>
-  <si>
-    <t>14.19</t>
-  </si>
-  <si>
     <t>dirt</t>
-  </si>
-  <si>
-    <t>Sherry</t>
-  </si>
-  <si>
-    <t>large</t>
-  </si>
-  <si>
-    <t>3.42</t>
-  </si>
-  <si>
-    <t>Jerry</t>
-  </si>
-  <si>
-    <t>medium</t>
-  </si>
-  <si>
-    <t>2.52</t>
-  </si>
-  <si>
-    <t>Terry</t>
-  </si>
-  <si>
-    <t>extra large</t>
-  </si>
-  <si>
-    <t>4.24</t>
-  </si>
-  <si>
-    <t>Personalize: Fill / extend tables</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="0"/>
-      <sz val="11"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
-      <b val="1"/>
-      <color rgb="FFC00000"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.7999816888943144"/>
-        <bgColor theme="6" tint="0.7999816888943144"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor theme="6" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
     <fill>
@@ -153,13 +109,13 @@
     <border>
       <left/>
       <right style="thin">
-        <color theme="3" tint="0.7999816888943144"/>
+        <color theme="3" tint="0.79998168889431442"/>
       </right>
       <top style="thin">
-        <color theme="6" tint="0.3999755851924192"/>
+        <color theme="6" tint="0.39997558519241921"/>
       </top>
       <bottom style="thin">
-        <color theme="6" tint="0.3999755851924192"/>
+        <color theme="6" tint="0.39997558519241921"/>
       </bottom>
       <diagonal/>
     </border>
@@ -169,10 +125,10 @@
       </left>
       <right/>
       <top style="thin">
-        <color theme="6" tint="0.3999755851924192"/>
+        <color theme="6" tint="0.39997558519241921"/>
       </top>
       <bottom style="thin">
-        <color theme="6" tint="0.3999755851924192"/>
+        <color theme="6" tint="0.39997558519241921"/>
       </bottom>
       <diagonal/>
     </border>
@@ -182,10 +138,10 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color theme="6" tint="0.3999755851924192"/>
+        <color theme="6" tint="0.39997558519241921"/>
       </top>
       <bottom style="thin">
-        <color theme="6" tint="0.3999755851924192"/>
+        <color theme="6" tint="0.39997558519241921"/>
       </bottom>
       <diagonal/>
     </border>
@@ -225,7 +181,7 @@
       </right>
       <top/>
       <bottom style="thin">
-        <color theme="6" tint="0.3999755851924192"/>
+        <color theme="6" tint="0.39997558519241921"/>
       </bottom>
       <diagonal/>
     </border>
@@ -236,7 +192,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color theme="6" tint="0.3999755851924192"/>
+        <color theme="6" tint="0.39997558519241921"/>
       </bottom>
       <diagonal/>
     </border>
@@ -244,10 +200,10 @@
       <left/>
       <right/>
       <top style="thin">
-        <color theme="6" tint="0.3999755851924192"/>
+        <color theme="6" tint="0.39997558519241921"/>
       </top>
       <bottom style="thin">
-        <color theme="6" tint="0.3999755851924192"/>
+        <color theme="6" tint="0.39997558519241921"/>
       </bottom>
       <diagonal/>
     </border>
@@ -256,7 +212,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color theme="6" tint="0.3999755851924192"/>
+        <color theme="6" tint="0.39997558519241921"/>
       </bottom>
       <diagonal/>
     </border>
@@ -266,7 +222,7 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color theme="6" tint="0.3999755851924192"/>
+        <color theme="6" tint="0.39997558519241921"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -277,7 +233,7 @@
       </left>
       <right/>
       <top style="thin">
-        <color theme="6" tint="0.3999755851924192"/>
+        <color theme="6" tint="0.39997558519241921"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -285,10 +241,10 @@
     <border>
       <left/>
       <right style="thin">
-        <color theme="3" tint="0.7999816888943144"/>
+        <color theme="3" tint="0.79998168889431442"/>
       </right>
       <top style="thin">
-        <color theme="6" tint="0.3999755851924192"/>
+        <color theme="6" tint="0.39997558519241921"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -297,108 +253,84 @@
       <left/>
       <right/>
       <top style="thin">
-        <color theme="6" tint="0.3999755851924192"/>
+        <color theme="6" tint="0.39997558519241921"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="3" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="3" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="4" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="23">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="7" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="9" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="9" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="10" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="11" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="12" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="13" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="14" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="8" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <font>
-        <name val="Arial Narrow"/>
-        <b val="1"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <condense val="0"/>
-        <color theme="0"/>
-        <extend val="0"/>
-        <sz val="11"/>
-        <vertAlign val="baseline"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="6"/>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top"/>
-    </dxf>
     <dxf>
       <border outline="0">
         <left style="thin">
@@ -411,27 +343,47 @@
           <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color theme="6" tint="0.3999755851924192"/>
+          <color theme="6" tint="0.39997558519241921"/>
         </bottom>
-        <diagonal/>
       </border>
     </dxf>
     <dxf>
       <font>
-        <name val="Arial Narrow"/>
+        <b/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <condense val="0"/>
-        <color theme="1"/>
-        <extend val="0"/>
+        <vertAlign val="baseline"/>
         <sz val="11"/>
-        <vertAlign val="baseline"/>
+        <color theme="0"/>
+        <name val="Arial Narrow"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="6" tint="0.7999816888943144"/>
-          <bgColor theme="6" tint="0.7999816888943144"/>
+          <fgColor theme="6"/>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial Narrow"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom"/>
@@ -439,67 +391,65 @@
         <left/>
         <right/>
         <top style="thin">
-          <color theme="6" tint="0.3999755851924192"/>
+          <color theme="6" tint="0.39997558519241921"/>
         </top>
         <bottom style="thin">
-          <color theme="6" tint="0.3999755851924192"/>
+          <color theme="6" tint="0.39997558519241921"/>
         </bottom>
-        <diagonal/>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
       <font>
-        <name val="Arial Narrow"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <condense val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
         <color theme="1"/>
-        <extend val="0"/>
-        <sz val="11"/>
-        <vertAlign val="baseline"/>
+        <name val="Arial Narrow"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="6" tint="0.7999816888943144"/>
-          <bgColor theme="6" tint="0.7999816888943144"/>
+          <fgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom"/>
       <border>
         <left/>
         <right style="thin">
-          <color theme="3" tint="0.7999816888943144"/>
+          <color theme="3" tint="0.79998168889431442"/>
         </right>
         <top style="thin">
-          <color theme="6" tint="0.3999755851924192"/>
+          <color theme="6" tint="0.39997558519241921"/>
         </top>
         <bottom style="thin">
-          <color theme="6" tint="0.3999755851924192"/>
+          <color theme="6" tint="0.39997558519241921"/>
         </bottom>
-        <diagonal/>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
       <font>
-        <name val="Arial Narrow"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <condense val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
         <color theme="1"/>
-        <extend val="0"/>
-        <sz val="11"/>
-        <vertAlign val="baseline"/>
+        <name val="Arial Narrow"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="6" tint="0.7999816888943144"/>
-          <bgColor theme="6" tint="0.7999816888943144"/>
+          <fgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom"/>
@@ -509,32 +459,31 @@
         </left>
         <right/>
         <top style="thin">
-          <color theme="6" tint="0.3999755851924192"/>
+          <color theme="6" tint="0.39997558519241921"/>
         </top>
         <bottom style="thin">
-          <color theme="6" tint="0.3999755851924192"/>
+          <color theme="6" tint="0.39997558519241921"/>
         </bottom>
-        <diagonal/>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
       <font>
-        <name val="Arial Narrow"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <condense val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
         <color theme="1"/>
-        <extend val="0"/>
-        <sz val="11"/>
-        <vertAlign val="baseline"/>
+        <name val="Arial Narrow"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="6" tint="0.7999816888943144"/>
-          <bgColor theme="6" tint="0.7999816888943144"/>
+          <fgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom"/>
@@ -544,12 +493,11 @@
           <color indexed="64"/>
         </right>
         <top style="thin">
-          <color theme="6" tint="0.3999755851924192"/>
+          <color theme="6" tint="0.39997558519241921"/>
         </top>
         <bottom style="thin">
-          <color theme="6" tint="0.3999755851924192"/>
+          <color theme="6" tint="0.39997558519241921"/>
         </bottom>
-        <diagonal/>
         <vertical/>
         <horizontal/>
       </border>
@@ -559,21 +507,9 @@
         <left/>
         <right/>
         <top style="thin">
-          <color theme="6" tint="0.3999755851924192"/>
+          <color theme="6" tint="0.39997558519241921"/>
         </top>
         <bottom/>
-        <diagonal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="6" tint="0.3999755851924192"/>
-        </bottom>
-        <diagonal/>
       </border>
     </dxf>
     <dxf>
@@ -588,34 +524,51 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <diagonal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </bottom>
       </border>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table3" headerRowBorderDxfId="7" headerRowCount="1" id="1" name="Table3" ref="D2:G7" tableBorderDxfId="8" totalsRowBorderDxfId="6" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="D2:G7" totalsRowShown="0" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="D2:G7"/>
   <tableColumns count="4">
-    <tableColumn dataDxfId="5" id="1" name="Client"/>
-    <tableColumn dataDxfId="4" id="2" name="#  scoops"/>
-    <tableColumn dataDxfId="3" id="3" name="flavor"/>
-    <tableColumn dataDxfId="2" id="4" name="Price (USD)"/>
+    <tableColumn id="1" name="Client" dataDxfId="5"/>
+    <tableColumn id="2" name="#  scoops" dataDxfId="4"/>
+    <tableColumn id="3" name="flavor" dataDxfId="3"/>
+    <tableColumn id="4" name="Price (USD)" dataDxfId="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table4" headerRowCount="1" headerRowDxfId="0" id="2" name="Table4" ref="B2:B5" tableBorderDxfId="1" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table4" displayName="Table4" ref="B2:B5" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="B2:B5"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Flavors"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -881,138 +834,91 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D3" sqref="D3:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="9.140625"/>
-    <col customWidth="1" max="2" min="2" style="13" width="9.85546875"/>
-    <col customWidth="1" max="3" min="3" style="13" width="10.140625"/>
-    <col customWidth="1" max="4" min="4" style="13" width="10.140625"/>
-    <col customWidth="1" max="5" min="5" style="13" width="12.28515625"/>
-    <col customWidth="1" max="6" min="6" style="13" width="13.5703125"/>
-    <col customWidth="1" max="7" min="7" style="13" width="16.85546875"/>
-    <col customWidth="1" max="9" min="8" style="1" width="9.140625"/>
-    <col customWidth="1" max="16384" min="10" style="1" width="9.140625"/>
+    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="12" customWidth="1"/>
+    <col min="3" max="4" width="10.140625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="12" customWidth="1"/>
+    <col min="8" max="11" width="9.140625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="F1" s="8" t="n"/>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F1" s="8"/>
     </row>
-    <row r="2" spans="1:7">
-      <c r="B2" s="23" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="11" t="n"/>
-      <c r="B3" s="15" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="10"/>
+      <c r="B3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="10" t="n"/>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="14"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="15"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="15" t="s">
-        <v>8</v>
-      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="14"/>
     </row>
-    <row r="4" spans="1:7">
-      <c r="B4" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="6" t="n">
-        <v>20</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>12</v>
-      </c>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D6" s="7"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="15"/>
     </row>
-    <row r="5" spans="1:7">
-      <c r="B5" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>16</v>
-      </c>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D7" s="17"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="20"/>
     </row>
-    <row r="6" spans="1:7">
-      <c r="D6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="D7" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="19" t="n">
-        <v>4</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="B9" s="12" t="s">
-        <v>23</v>
-      </c>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="11"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <tableParts count="2">
     <tablePart r:id="rId1"/>

</xml_diff>